<commit_message>
Ensure calculated values appear with measurements on the same page
Update template creation script to associate calculated questions with the 'Mérések' (Measurements) block, ensuring they are displayed alongside their corresponding measurements and resolving progression issues.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 69c03b3f-dab7-4110-9b25-5f5d4e1d7562
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/81db43ca-5fb4-437b-bfda-4fcd8b7b2002/69c03b3f-dab7-4110-9b25-5f5d4e1d7562/ZT9cPru
</commit_message>
<xml_diff>
--- a/COMPREHENSIVE-TEMPLATE-FULL.xlsx
+++ b/COMPREHENSIVE-TEMPLATE-FULL.xlsx
@@ -1064,7 +1064,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>A + B + C</t>
+          <t>m1 + m2 + m3</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -1084,11 +1084,11 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Számítások</t>
+          <t>Mérések</t>
         </is>
       </c>
       <c r="L9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Berechnungen</t>
+          <t>Messungen</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">

</xml_diff>